<commit_message>
Laborator 1 - MenuDataModel + PaymentType - SonarLint
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenagrigorescu/Anul3/Semestru2/VVSS/CheckLists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenagrigorescu/Anul3/Semestru2/VVSS/PizzaShop/Docs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F30E39C-C007-FA48-9AAF-DAFE860DC30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7056197F-FF63-574C-8946-5DCF2B783421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26440" windowHeight="16260" tabRatio="650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -144,13 +144,104 @@
   </si>
   <si>
     <t>Ghinea Bogdan-Florin</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>Bucataria unde se alfa maestrul pizzar se poate inchide doar daca nu mai exista clienti.</t>
+  </si>
+  <si>
+    <t>La initializarea sistemului bucataria e deschisa dar nu exista niciun client</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>O masa poate fi eliberata la cerere, doar dupa achitarea comenzii.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nu este mentionat daca clientul poate sa faca mai multe comenzi </t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Aplicatia permite plasarea si onorarea comenzilor de pizza</t>
+  </si>
+  <si>
+    <t>Nu se specifica metoda prin care sunt luate comenzile (telefonic, aplicatie web etc.)</t>
+  </si>
+  <si>
+    <t>jumatate de ora</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>MenuDataModel</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>KitchenGUI class</t>
+  </si>
+  <si>
+    <t>Nu ar trebui legata direct de Main, ci de o clasa de tip Controller</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>Nu exista mecanisme de error handling in momentul in care un utilizator plateste cu un card care nu are destui bani sau cand clientul introduce o cantitate negativa in comanda sau un item inexistent</t>
+  </si>
+  <si>
+    <t>Nu se pune problema de cantitate in momentul incarcarii meniului (la initializarea sistemului) si in OrderGUI nu ar trebui sa exista relatie directa cu un obiect de tip service</t>
+  </si>
+  <si>
+    <t>MenuRepository</t>
+  </si>
+  <si>
+    <t>menuItemProperty (L22) - metoda nu este corect denumita; ar trebui folosit getter, adica getMenuItemProperty</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getMenuItem poate returna valori null si ca urmare lista de menu items poate contine null </t>
+  </si>
+  <si>
+    <t>PizzaService</t>
+  </si>
+  <si>
+    <t>numele pentru lista de plati esti nesugestiv denumita (l), ar trebui sa se numeasca payments (L32)</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>PaymentAlert</t>
+  </si>
+  <si>
+    <t>Optional&lt;ButtonType&gt; result = paymentAlert.showAndWait();
+        if (result.get() == cardPayment) - daca nu se verifica cu isPresent() valoarea din Optional, se va arunca NoSuchElementException</t>
+  </si>
+  <si>
+    <t>MenuDataModel class si OrdersGUI class</t>
+  </si>
+  <si>
+    <t>MenuDataModel + PaymentType - SonarLint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +318,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
     </font>
   </fonts>
   <fills count="5">
@@ -328,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -358,6 +466,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -400,7 +512,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,40 +822,41 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="73.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8.83203125" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
     <col min="10" max="10" width="14.5" style="6" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -752,57 +865,69 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="17">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="16">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -816,33 +941,51 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="32">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="32">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="32">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -851,7 +994,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -860,7 +1003,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -869,7 +1012,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -878,7 +1021,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -887,7 +1030,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -896,7 +1039,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -905,7 +1048,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -914,7 +1057,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -923,7 +1066,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -932,7 +1075,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -941,7 +1084,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -950,7 +1093,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -959,12 +1102,14 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -985,41 +1130,42 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.83203125" style="6"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1028,57 +1174,69 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="17">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1092,33 +1250,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="64">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="32">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="80">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1127,7 +1301,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1136,7 +1310,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1145,7 +1319,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1154,7 +1328,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1163,7 +1337,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1172,7 +1346,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1181,7 +1355,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1190,7 +1364,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1199,7 +1373,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1208,7 +1382,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1217,7 +1391,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1226,7 +1400,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1235,7 +1409,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1244,12 +1418,22 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="C30" s="39">
+        <v>45370</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1273,39 +1457,39 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="77" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="8.83203125" style="6"/>
     <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1314,57 +1498,69 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="17">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1378,42 +1574,66 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="16">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="48">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1422,7 +1642,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1431,7 +1651,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1440,7 +1660,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1449,7 +1669,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1458,7 +1678,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1467,7 +1687,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1476,7 +1696,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1485,7 +1705,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1494,7 +1714,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1503,7 +1723,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1512,7 +1732,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1521,7 +1741,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1530,7 +1750,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1539,7 +1759,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1548,7 +1768,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1557,7 +1777,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1566,12 +1786,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1595,10 +1817,10 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -1611,24 +1833,24 @@
     <col min="10" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="23" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1637,59 +1859,59 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="21" t="s">
         <v>35</v>
       </c>
       <c r="J5" s="3">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1706,7 +1928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1715,7 +1937,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1725,7 +1947,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1735,7 +1957,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1745,7 +1967,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1755,7 +1977,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1765,7 +1987,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1775,7 +1997,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1785,7 +2007,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1795,7 +2017,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1805,7 +2027,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1815,7 +2037,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1825,7 +2047,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1835,7 +2057,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1845,7 +2067,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1855,7 +2077,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1865,7 +2087,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1875,7 +2097,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1885,7 +2107,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1895,7 +2117,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1905,7 +2127,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1915,12 +2137,12 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="33" t="s">
+    <row r="32" spans="2:6">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>